<commit_message>
Update the revision history and reference table in HSI document and updating the HSI review sheet Signed-off-by: AmiraZaher <amirazaher96@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/HSI/HSI_Review.xlsx
+++ b/Input documents/HSI/HSI_Review.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Software Engineering\Blender_Project\Input documents\HSI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Introduction " sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Cross review points " sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Introduction " sheetId="1" r:id="rId1"/>
+    <sheet name="Cross review points " sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_Toc30697436" vbProcedure="false">'Cross review points '!$F$7</definedName>
+    <definedName name="_Toc30697436" localSheetId="1">'Cross review points '!$F$7</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -41,28 +45,28 @@
     <t xml:space="preserve">Ref Version </t>
   </si>
   <si>
-    <t xml:space="preserve">V1.2</t>
+    <t>V1.2</t>
   </si>
   <si>
     <t xml:space="preserve">Auther </t>
   </si>
   <si>
-    <t xml:space="preserve">Tarek Sharaby</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">History</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auther</t>
+    <t>Tarek Sharaby</t>
+  </si>
+  <si>
+    <t>Last update</t>
+  </si>
+  <si>
+    <t>24/01/2020</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Auther</t>
   </si>
   <si>
     <t xml:space="preserve">Date </t>
@@ -71,102 +75,102 @@
     <t xml:space="preserve">Change </t>
   </si>
   <si>
-    <t xml:space="preserve">T.Sharaby</t>
+    <t>T.Sharaby</t>
   </si>
   <si>
     <t xml:space="preserve">Initial creation </t>
   </si>
   <si>
-    <t xml:space="preserve">Entry Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detection version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page/Line/Section/Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open point : description of problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.Ali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V0.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 1</t>
+    <t>Entry Date</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Detection version</t>
+  </si>
+  <si>
+    <t>Name of file</t>
+  </si>
+  <si>
+    <t>Page/Line/Section/Entity</t>
+  </si>
+  <si>
+    <t>Open point : description of problem</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>29/01/2020</t>
+  </si>
+  <si>
+    <t>A.Ali</t>
+  </si>
+  <si>
+    <t>V0.1</t>
+  </si>
+  <si>
+    <t>HSI</t>
+  </si>
+  <si>
+    <t>Page 1</t>
   </si>
   <si>
     <t xml:space="preserve">Status of document must be changed from Draft to Proposed and then Released after accomplishing cross review on it. 
 I expect if cross review was done by another team member , the status of document should be Released. </t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All pages</t>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>All pages</t>
   </si>
   <si>
     <t xml:space="preserve">Redundancy in Version field besides Date in header table. </t>
   </si>
   <si>
-    <t xml:space="preserve">All</t>
+    <t>All</t>
   </si>
   <si>
     <t xml:space="preserve">There is no Reference table for the reference document , even HSI should have one and the reference is the customer Requirement for the product </t>
   </si>
   <si>
-    <t xml:space="preserve">Refused</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 5</t>
+    <t>Refused</t>
+  </si>
+  <si>
+    <t>Page 5</t>
   </si>
   <si>
     <t xml:space="preserve">System Block Diagram shall be updated to match customer specification defined in CRS , as there’s no mentioned specification states that there’s 3 LEDs  and the arrow connected between push button and Microcontroller should be an input not output. </t>
   </si>
   <si>
-    <t xml:space="preserve">Page 6</t>
+    <t>Page 6</t>
   </si>
   <si>
     <t xml:space="preserve">You could add a requirement ID to Pin Mode Representation section above the table , also there’s no block diagram added to the section 2.3 Speed Mode Block Diagram , if there’s no need for it , delete this section. </t>
   </si>
   <si>
-    <t xml:space="preserve">Page 7</t>
+    <t>Page 7</t>
   </si>
   <si>
     <t xml:space="preserve">In Section 3 : Functional Requirements , you need to change the requirement ID for all the mentioned requirements and Implementation must be by HW as HSI document scope is only HW requirements.
 - Need to review HSI requirements again and add a related HW requirements from the system level prospective. </t>
   </si>
   <si>
-    <t xml:space="preserve">Open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V1.6</t>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>V1.6</t>
   </si>
   <si>
     <t xml:space="preserve">Version Date format in header table is different from the Date field in Release Table in page 2 , plaese apply a unique Date format for all date fields , also HSI document stands for Hardware Software Interface. </t>
@@ -195,16 +199,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY;@"/>
-    <numFmt numFmtId="166" formatCode="[$-409]General"/>
-    <numFmt numFmtId="167" formatCode="[$-409]M/D/YYYY"/>
-    <numFmt numFmtId="168" formatCode="@"/>
-    <numFmt numFmtId="169" formatCode="[$-409]MM/DD/YY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]General"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yyyy"/>
+    <numFmt numFmtId="167" formatCode="[$-409]mm/dd/yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -213,22 +215,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -236,7 +223,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -258,6 +245,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -291,103 +285,149 @@
     </fill>
   </fills>
   <borders count="11">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -403,215 +443,160 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in Accent3" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Normal 3 2" xfId="20"/>
-    <cellStyle name="Normal 4" xfId="21"/>
-    <cellStyle name="Excel Built-in Accent3" xfId="22"/>
+    <cellStyle name="Normal 3 2" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF808080"/>
+        <color rgb="FFFBE5D6"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF1F4E79"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAE3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF385724"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color rgb="FF535353"/>
       </font>
@@ -623,41 +608,18 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF385724"/>
+        <color rgb="FF808080"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FF1F4E79"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAE3F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FFFBE5D6"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FFF2F2F2"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -716,223 +678,500 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F4E79"/>
       <rgbColor rgb="FF385724"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B2:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="5"/>
+      <c r="G12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="9" t="n">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
         <v>0.1</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
@@ -940,57 +1179,46 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:L1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="174.28"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
@@ -1019,7 +1247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
@@ -1046,7 +1274,7 @@
       </c>
       <c r="I2" s="22"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
@@ -1072,11 +1300,11 @@
         <v>33</v>
       </c>
       <c r="I3" s="22"/>
-      <c r="K3" s="0" t="s">
+      <c r="K3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>26</v>
       </c>
@@ -1102,11 +1330,11 @@
         <v>33</v>
       </c>
       <c r="I4" s="22"/>
-      <c r="K4" s="0" t="s">
+      <c r="K4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>26</v>
       </c>
@@ -1133,7 +1361,7 @@
       </c>
       <c r="I5" s="22"/>
     </row>
-    <row r="6" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
@@ -1160,7 +1388,7 @@
       </c>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
@@ -1186,12 +1414,12 @@
         <v>45</v>
       </c>
       <c r="I7" s="20"/>
-      <c r="K7" s="0" t="s">
+      <c r="K7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="n">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
         <v>44014</v>
       </c>
       <c r="B8" s="18" t="s">
@@ -1209,17 +1437,19 @@
       <c r="F8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="22"/>
+      <c r="G8" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H8" s="22" t="s">
         <v>45</v>
       </c>
       <c r="I8" s="20"/>
-      <c r="K8" s="0" t="s">
+      <c r="K8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="n">
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
         <v>44014</v>
       </c>
       <c r="B9" s="18" t="s">
@@ -1237,14 +1467,16 @@
       <c r="F9" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="22"/>
+      <c r="G9" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H9" s="22" t="s">
         <v>45</v>
       </c>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="n">
+    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
         <v>44014</v>
       </c>
       <c r="B10" s="18" t="s">
@@ -1262,13 +1494,15 @@
       <c r="F10" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H10" s="22" t="s">
         <v>45</v>
       </c>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -1278,14 +1512,14 @@
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="20"/>
-      <c r="K11" s="0" t="s">
+      <c r="K11" t="s">
         <v>50</v>
       </c>
-      <c r="L11" s="0" t="s">
+      <c r="L11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -1295,14 +1529,14 @@
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
       <c r="I12" s="20"/>
-      <c r="K12" s="0" t="s">
+      <c r="K12" t="s">
         <v>52</v>
       </c>
-      <c r="L12" s="0" t="s">
+      <c r="L12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -1313,7 +1547,7 @@
       <c r="H13" s="22"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -1324,7 +1558,7 @@
       <c r="H14" s="22"/>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -1335,7 +1569,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -1346,7 +1580,7 @@
       <c r="H16" s="22"/>
       <c r="I16" s="32"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -1357,7 +1591,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="32"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
       <c r="B18" s="28"/>
       <c r="C18" s="29"/>
@@ -1368,7 +1602,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="32"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
       <c r="B19" s="28"/>
       <c r="C19" s="29"/>
@@ -1379,7 +1613,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="32"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="27"/>
       <c r="B20" s="28"/>
       <c r="C20" s="29"/>
@@ -1390,7 +1624,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="32"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="28"/>
       <c r="C21" s="29"/>
@@ -1401,7 +1635,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="32"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
       <c r="B22" s="28"/>
       <c r="C22" s="29"/>
@@ -1412,7 +1646,7 @@
       <c r="H22" s="22"/>
       <c r="I22" s="32"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
@@ -1423,7 +1657,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="32"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="28"/>
       <c r="C24" s="29"/>
@@ -1434,7 +1668,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="32"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
@@ -1445,7 +1679,7 @@
       <c r="H25" s="22"/>
       <c r="I25" s="32"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
@@ -1456,7 +1690,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="32"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="28"/>
       <c r="C27" s="29"/>
@@ -1467,7 +1701,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="32"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
@@ -1478,7 +1712,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="32"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
@@ -1489,7 +1723,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="32"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
@@ -1500,7 +1734,7 @@
       <c r="H30" s="22"/>
       <c r="I30" s="32"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
       <c r="B31" s="28"/>
       <c r="C31" s="28"/>
@@ -1511,7 +1745,7 @@
       <c r="H31" s="22"/>
       <c r="I31" s="32"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="29"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
@@ -1522,7 +1756,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="29"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
@@ -1533,7 +1767,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="27"/>
       <c r="B34" s="28"/>
       <c r="C34" s="28"/>
@@ -1544,7 +1778,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="29"/>
       <c r="B35" s="29"/>
       <c r="C35" s="29"/>
@@ -1555,7 +1789,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="29"/>
       <c r="B36" s="29"/>
       <c r="C36" s="29"/>
@@ -1566,7 +1800,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="29"/>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
@@ -1577,7 +1811,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="29"/>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
@@ -1588,7 +1822,7 @@
       <c r="H38" s="22"/>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="29"/>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
@@ -1599,7 +1833,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="29"/>
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
@@ -1610,7 +1844,7 @@
       <c r="H40" s="22"/>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="29"/>
       <c r="B41" s="29"/>
       <c r="C41" s="29"/>
@@ -1621,7 +1855,7 @@
       <c r="H41" s="22"/>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="29"/>
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
@@ -1632,7 +1866,7 @@
       <c r="H42" s="22"/>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="29"/>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>
@@ -1643,7 +1877,7 @@
       <c r="H43" s="22"/>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="29"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
@@ -1654,7 +1888,7 @@
       <c r="H44" s="22"/>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="29"/>
       <c r="B45" s="29"/>
       <c r="C45" s="29"/>
@@ -1665,7 +1899,7 @@
       <c r="H45" s="22"/>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="29"/>
       <c r="B46" s="29"/>
       <c r="C46" s="29"/>
@@ -1676,7 +1910,7 @@
       <c r="H46" s="22"/>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="29"/>
       <c r="B47" s="29"/>
       <c r="C47" s="29"/>
@@ -1687,47 +1921,41 @@
       <c r="H47" s="22"/>
       <c r="I47" s="32"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>#ref!</formula>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>#ref!</formula>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>#ref!</formula>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1 G8:G1047" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1 G11:G1047">
       <formula1>$K$4:$K$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H1047" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1047">
       <formula1>$K$7:$K$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G7" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G10">
       <formula1>$K$3:$K$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>